<commit_message>
Voici la version finale de notre solution du projet de fin d'année ING1 GM pour le problème d'orientation. Signature: Equipe_7
</commit_message>
<xml_diff>
--- a/Annexes/jeu_donnees.xlsx
+++ b/Annexes/jeu_donnees.xlsx
@@ -5,20 +5,20 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Desktop\ING1\projet_fin_annee\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Desktop\ING1\projet_fin_annee\projet_fin_d_annee\Annexes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADAFB36D-4CA7-49AF-8D4A-15814F71E0CE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F735EAE-D694-47C0-812C-4ABB8E57BA5B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="5" xr2:uid="{4CFD88F8-A435-406B-86AE-50E0EF38730A}"/>
   </bookViews>
   <sheets>
     <sheet name="GMI" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet3" sheetId="5" r:id="rId2"/>
-    <sheet name="GMF" sheetId="2" r:id="rId3"/>
-    <sheet name="GM_résultats" sheetId="3" r:id="rId4"/>
-    <sheet name="MI" sheetId="4" r:id="rId5"/>
-    <sheet name="MF" sheetId="7" r:id="rId6"/>
+    <sheet name="GMF" sheetId="2" r:id="rId2"/>
+    <sheet name="GM_résultats" sheetId="3" r:id="rId3"/>
+    <sheet name="MI" sheetId="4" r:id="rId4"/>
+    <sheet name="MF" sheetId="7" r:id="rId5"/>
+    <sheet name="GI" sheetId="8" r:id="rId6"/>
     <sheet name="Sheet4" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1154" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1314" uniqueCount="278">
   <si>
     <t>Identifiant</t>
   </si>
@@ -634,13 +634,244 @@
   </si>
   <si>
     <t>Actuariat,MMF</t>
+  </si>
+  <si>
+    <t>Brisset</t>
+  </si>
+  <si>
+    <t>Landry</t>
+  </si>
+  <si>
+    <t>Dard</t>
+  </si>
+  <si>
+    <t>Touzet</t>
+  </si>
+  <si>
+    <t>Aubin</t>
+  </si>
+  <si>
+    <t>Latour</t>
+  </si>
+  <si>
+    <t>Léna</t>
+  </si>
+  <si>
+    <t>Demoulin</t>
+  </si>
+  <si>
+    <t>Agathe</t>
+  </si>
+  <si>
+    <t>Elite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Charlie </t>
+  </si>
+  <si>
+    <t>Ory</t>
+  </si>
+  <si>
+    <t>Miot</t>
+  </si>
+  <si>
+    <t>Marti</t>
+  </si>
+  <si>
+    <t>Mael</t>
+  </si>
+  <si>
+    <t>Patry</t>
+  </si>
+  <si>
+    <t>Marcel</t>
+  </si>
+  <si>
+    <t>Charlie</t>
+  </si>
+  <si>
+    <t>Besson</t>
+  </si>
+  <si>
+    <t>Florin</t>
+  </si>
+  <si>
+    <t>Gabin</t>
+  </si>
+  <si>
+    <t>Delaire</t>
+  </si>
+  <si>
+    <t>Isac</t>
+  </si>
+  <si>
+    <t>Sylvie</t>
+  </si>
+  <si>
+    <t>La farge</t>
+  </si>
+  <si>
+    <t>Léon</t>
+  </si>
+  <si>
+    <t>Dion</t>
+  </si>
+  <si>
+    <t>ICC</t>
+  </si>
+  <si>
+    <t>Milon</t>
+  </si>
+  <si>
+    <t>Roth</t>
+  </si>
+  <si>
+    <t>Mia</t>
+  </si>
+  <si>
+    <t>Penot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Julia </t>
+  </si>
+  <si>
+    <t>Le Breton</t>
+  </si>
+  <si>
+    <t>Anne</t>
+  </si>
+  <si>
+    <t>Perin</t>
+  </si>
+  <si>
+    <t>Dreux</t>
+  </si>
+  <si>
+    <t>Mathis</t>
+  </si>
+  <si>
+    <t>Varlet</t>
+  </si>
+  <si>
+    <t>Dumon</t>
+  </si>
+  <si>
+    <t>Maxence</t>
+  </si>
+  <si>
+    <t>Pirot</t>
+  </si>
+  <si>
+    <t>Livio</t>
+  </si>
+  <si>
+    <t>Delphine</t>
+  </si>
+  <si>
+    <t>Hugo</t>
+  </si>
+  <si>
+    <t>Loret</t>
+  </si>
+  <si>
+    <t>Yanis</t>
+  </si>
+  <si>
+    <t>Hermain</t>
+  </si>
+  <si>
+    <t>Inaya</t>
+  </si>
+  <si>
+    <t>Fabry</t>
+  </si>
+  <si>
+    <t>Jeanne</t>
+  </si>
+  <si>
+    <t>Vienne</t>
+  </si>
+  <si>
+    <t>De valois</t>
+  </si>
+  <si>
+    <t>Fouet</t>
+  </si>
+  <si>
+    <t>Chistiane</t>
+  </si>
+  <si>
+    <t>Talbot</t>
+  </si>
+  <si>
+    <t>Nicol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alma </t>
+  </si>
+  <si>
+    <t>Allier</t>
+  </si>
+  <si>
+    <t>Denise</t>
+  </si>
+  <si>
+    <t>Lariot</t>
+  </si>
+  <si>
+    <t>Eden</t>
+  </si>
+  <si>
+    <t>Hery</t>
+  </si>
+  <si>
+    <t>Isaac</t>
+  </si>
+  <si>
+    <t>INEM</t>
+  </si>
+  <si>
+    <t>Tardy</t>
+  </si>
+  <si>
+    <t>Baptiste</t>
+  </si>
+  <si>
+    <t>Chanel</t>
+  </si>
+  <si>
+    <t>Fauveau</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alexandre </t>
+  </si>
+  <si>
+    <t>Barry</t>
+  </si>
+  <si>
+    <t>Suzane</t>
+  </si>
+  <si>
+    <t>Nicole</t>
+  </si>
+  <si>
+    <t>Breuil</t>
+  </si>
+  <si>
+    <t>Madeleine</t>
+  </si>
+  <si>
+    <t>CS</t>
+  </si>
+  <si>
+    <t>VC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -677,8 +908,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="13">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -747,6 +992,16 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -787,7 +1042,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -801,8 +1056,10 @@
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="5"/>
@@ -820,8 +1077,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" xfId="14"/>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" xfId="13"/>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="15">
     <cellStyle name="20% - Accent1" xfId="4" builtinId="30"/>
     <cellStyle name="20% - Accent2" xfId="6" builtinId="34"/>
     <cellStyle name="20% - Accent4" xfId="10" builtinId="42"/>
@@ -832,7 +1091,9 @@
     <cellStyle name="Accent2" xfId="5" builtinId="33"/>
     <cellStyle name="Accent4" xfId="9" builtinId="41"/>
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="13" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Neutral" xfId="14" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="3" builtinId="10"/>
   </cellStyles>
@@ -1148,8 +1409,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FAB5699-3625-410F-8E4D-225DFE3C15A7}">
   <dimension ref="A1:L52"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="85" zoomScaleNormal="133" workbookViewId="0">
-      <selection activeCell="J1" activeCellId="1" sqref="A1:C52 J1:L52"/>
+    <sheetView zoomScale="85" zoomScaleNormal="133" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1199,6 +1460,9 @@
       <c r="K1" s="12" t="s">
         <v>181</v>
       </c>
+      <c r="L1" s="12" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2">
@@ -1229,11 +1493,11 @@
         <v>20</v>
       </c>
       <c r="J2">
-        <f>AVERAGE(D2:I2)</f>
+        <f t="shared" ref="J2:J33" si="0">AVERAGE(D2:I2)</f>
         <v>19.041666666666668</v>
       </c>
       <c r="K2">
-        <f>5*D2 +4.5*E2 +3*F2+3*G2+2.5*H2+2*I2</f>
+        <f t="shared" ref="K2:K33" si="1">5*D2 +4.5*E2 +3*F2+3*G2+2.5*H2+2*I2</f>
         <v>378.875</v>
       </c>
       <c r="L2" t="s">
@@ -1269,11 +1533,11 @@
         <v>20</v>
       </c>
       <c r="J3">
-        <f>AVERAGE(D3:I3)</f>
+        <f t="shared" si="0"/>
         <v>18.458333333333332</v>
       </c>
       <c r="K3">
-        <f>5*D3 +4.5*E3 +3*F3+3*G3+2.5*H3+2*I3</f>
+        <f t="shared" si="1"/>
         <v>367.375</v>
       </c>
       <c r="L3" t="s">
@@ -1309,11 +1573,11 @@
         <v>19.5</v>
       </c>
       <c r="J4">
-        <f>AVERAGE(D4:I4)</f>
+        <f t="shared" si="0"/>
         <v>17.75</v>
       </c>
       <c r="K4">
-        <f>5*D4 +4.5*E4 +3*F4+3*G4+2.5*H4+2*I4</f>
+        <f t="shared" si="1"/>
         <v>358.75</v>
       </c>
       <c r="L4" t="s">
@@ -1349,11 +1613,11 @@
         <v>19</v>
       </c>
       <c r="J5">
-        <f>AVERAGE(D5:I5)</f>
+        <f t="shared" si="0"/>
         <v>17.383333333333333</v>
       </c>
       <c r="K5">
-        <f>5*D5 +4.5*E5 +3*F5+3*G5+2.5*H5+2*I5</f>
+        <f t="shared" si="1"/>
         <v>346.25</v>
       </c>
       <c r="L5" t="s">
@@ -1389,11 +1653,11 @@
         <v>17.75</v>
       </c>
       <c r="J6">
-        <f>AVERAGE(D6:I6)</f>
+        <f t="shared" si="0"/>
         <v>17.375</v>
       </c>
       <c r="K6">
-        <f>5*D6 +4.5*E6 +3*F6+3*G6+2.5*H6+2*I6</f>
+        <f t="shared" si="1"/>
         <v>345.5</v>
       </c>
       <c r="L6" t="s">
@@ -1429,11 +1693,11 @@
         <v>20</v>
       </c>
       <c r="J7">
-        <f>AVERAGE(D7:I7)</f>
+        <f t="shared" si="0"/>
         <v>16.400000000000002</v>
       </c>
       <c r="K7">
-        <f>5*D7 +4.5*E7 +3*F7+3*G7+2.5*H7+2*I7</f>
+        <f t="shared" si="1"/>
         <v>321.375</v>
       </c>
       <c r="L7" t="s">
@@ -1469,11 +1733,11 @@
         <v>15</v>
       </c>
       <c r="J8">
-        <f>AVERAGE(D8:I8)</f>
+        <f t="shared" si="0"/>
         <v>15.875</v>
       </c>
       <c r="K8">
-        <f>5*D8 +4.5*E8 +3*F8+3*G8+2.5*H8+2*I8</f>
+        <f t="shared" si="1"/>
         <v>321</v>
       </c>
       <c r="L8" t="s">
@@ -1509,11 +1773,11 @@
         <v>16.5</v>
       </c>
       <c r="J9">
-        <f>AVERAGE(D9:I9)</f>
+        <f t="shared" si="0"/>
         <v>15.833333333333334</v>
       </c>
       <c r="K9">
-        <f>5*D9 +4.5*E9 +3*F9+3*G9+2.5*H9+2*I9</f>
+        <f t="shared" si="1"/>
         <v>320.25</v>
       </c>
       <c r="L9" t="s">
@@ -1549,11 +1813,11 @@
         <v>15.8</v>
       </c>
       <c r="J10">
-        <f>AVERAGE(D10:I10)</f>
+        <f t="shared" si="0"/>
         <v>15.591666666666667</v>
       </c>
       <c r="K10">
-        <f>5*D10 +4.5*E10 +3*F10+3*G10+2.5*H10+2*I10</f>
+        <f t="shared" si="1"/>
         <v>318.85000000000002</v>
       </c>
       <c r="L10" t="s">
@@ -1589,11 +1853,11 @@
         <v>15</v>
       </c>
       <c r="J11">
-        <f>AVERAGE(D11:I11)</f>
+        <f t="shared" si="0"/>
         <v>15.625</v>
       </c>
       <c r="K11">
-        <f>5*D11 +4.5*E11 +3*F11+3*G11+2.5*H11+2*I11</f>
+        <f t="shared" si="1"/>
         <v>315.5</v>
       </c>
       <c r="L11" t="s">
@@ -1629,11 +1893,11 @@
         <v>14</v>
       </c>
       <c r="J12">
-        <f>AVERAGE(D12:I12)</f>
+        <f t="shared" si="0"/>
         <v>15.833333333333334</v>
       </c>
       <c r="K12">
-        <f>5*D12 +4.5*E12 +3*F12+3*G12+2.5*H12+2*I12</f>
+        <f t="shared" si="1"/>
         <v>312</v>
       </c>
       <c r="L12" t="s">
@@ -1669,11 +1933,11 @@
         <v>17</v>
       </c>
       <c r="J13">
-        <f>AVERAGE(D13:I13)</f>
+        <f t="shared" si="0"/>
         <v>15.333333333333334</v>
       </c>
       <c r="K13">
-        <f>5*D13 +4.5*E13 +3*F13+3*G13+2.5*H13+2*I13</f>
+        <f t="shared" si="1"/>
         <v>309.25</v>
       </c>
       <c r="L13" t="s">
@@ -1709,11 +1973,11 @@
         <v>17.899999999999999</v>
       </c>
       <c r="J14">
-        <f>AVERAGE(D14:I14)</f>
+        <f t="shared" si="0"/>
         <v>15.566666666666668</v>
       </c>
       <c r="K14">
-        <f>5*D14 +4.5*E14 +3*F14+3*G14+2.5*H14+2*I14</f>
+        <f t="shared" si="1"/>
         <v>304.92500000000001</v>
       </c>
       <c r="L14" t="s">
@@ -1749,11 +2013,11 @@
         <v>17</v>
       </c>
       <c r="J15">
-        <f>AVERAGE(D15:I15)</f>
+        <f t="shared" si="0"/>
         <v>14.958333333333334</v>
       </c>
       <c r="K15">
-        <f>5*D15 +4.5*E15 +3*F15+3*G15+2.5*H15+2*I15</f>
+        <f t="shared" si="1"/>
         <v>303.625</v>
       </c>
       <c r="L15" t="s">
@@ -1789,11 +2053,11 @@
         <v>15</v>
       </c>
       <c r="J16">
-        <f>AVERAGE(D16:I16)</f>
+        <f t="shared" si="0"/>
         <v>15.041666666666666</v>
       </c>
       <c r="K16">
-        <f>5*D16 +4.5*E16 +3*F16+3*G16+2.5*H16+2*I16</f>
+        <f t="shared" si="1"/>
         <v>303.25</v>
       </c>
       <c r="L16" t="s">
@@ -1829,11 +2093,11 @@
         <v>18.5</v>
       </c>
       <c r="J17">
-        <f>AVERAGE(D17:I17)</f>
+        <f t="shared" si="0"/>
         <v>15.833333333333334</v>
       </c>
       <c r="K17">
-        <f>5*D17 +4.5*E17 +3*F17+3*G17+2.5*H17+2*I17</f>
+        <f t="shared" si="1"/>
         <v>301.75</v>
       </c>
       <c r="L17" t="s">
@@ -1869,11 +2133,11 @@
         <v>12.5</v>
       </c>
       <c r="J18">
-        <f>AVERAGE(D18:I18)</f>
+        <f t="shared" si="0"/>
         <v>14.708333333333334</v>
       </c>
       <c r="K18">
-        <f>5*D18 +4.5*E18 +3*F18+3*G18+2.5*H18+2*I18</f>
+        <f t="shared" si="1"/>
         <v>300.75</v>
       </c>
       <c r="L18" t="s">
@@ -1909,11 +2173,11 @@
         <v>15</v>
       </c>
       <c r="J19">
-        <f>AVERAGE(D19:I19)</f>
+        <f t="shared" si="0"/>
         <v>15.25</v>
       </c>
       <c r="K19">
-        <f>5*D19 +4.5*E19 +3*F19+3*G19+2.5*H19+2*I19</f>
+        <f t="shared" si="1"/>
         <v>299.75</v>
       </c>
       <c r="L19" t="s">
@@ -1949,11 +2213,11 @@
         <v>10</v>
       </c>
       <c r="J20">
-        <f>AVERAGE(D20:I20)</f>
+        <f t="shared" si="0"/>
         <v>14.094999999999999</v>
       </c>
       <c r="K20">
-        <f>5*D20 +4.5*E20 +3*F20+3*G20+2.5*H20+2*I20</f>
+        <f t="shared" si="1"/>
         <v>297.47500000000002</v>
       </c>
       <c r="L20" t="s">
@@ -1989,11 +2253,11 @@
         <v>17.8</v>
       </c>
       <c r="J21">
-        <f>AVERAGE(D21:I21)</f>
+        <f t="shared" si="0"/>
         <v>14.258333333333333</v>
       </c>
       <c r="K21">
-        <f>5*D21 +4.5*E21 +3*F21+3*G21+2.5*H21+2*I21</f>
+        <f t="shared" si="1"/>
         <v>296.97500000000002</v>
       </c>
       <c r="L21" t="s">
@@ -2029,11 +2293,11 @@
         <v>16</v>
       </c>
       <c r="J22">
-        <f>AVERAGE(D22:I22)</f>
+        <f t="shared" si="0"/>
         <v>14.878333333333332</v>
       </c>
       <c r="K22">
-        <f>5*D22 +4.5*E22 +3*F22+3*G22+2.5*H22+2*I22</f>
+        <f t="shared" si="1"/>
         <v>294.81</v>
       </c>
       <c r="L22" t="s">
@@ -2069,11 +2333,11 @@
         <v>16.5</v>
       </c>
       <c r="J23">
-        <f>AVERAGE(D23:I23)</f>
+        <f t="shared" si="0"/>
         <v>15.125</v>
       </c>
       <c r="K23">
-        <f>5*D23 +4.5*E23 +3*F23+3*G23+2.5*H23+2*I23</f>
+        <f t="shared" si="1"/>
         <v>294.375</v>
       </c>
       <c r="L23" t="s">
@@ -2109,11 +2373,11 @@
         <v>18.5</v>
       </c>
       <c r="J24">
-        <f>AVERAGE(D24:I24)</f>
+        <f t="shared" si="0"/>
         <v>14.625</v>
       </c>
       <c r="K24">
-        <f>5*D24 +4.5*E24 +3*F24+3*G24+2.5*H24+2*I24</f>
+        <f t="shared" si="1"/>
         <v>292.5</v>
       </c>
       <c r="L24" t="s">
@@ -2149,11 +2413,11 @@
         <v>17</v>
       </c>
       <c r="J25">
-        <f>AVERAGE(D25:I25)</f>
+        <f t="shared" si="0"/>
         <v>14.583333333333334</v>
       </c>
       <c r="K25">
-        <f>5*D25 +4.5*E25 +3*F25+3*G25+2.5*H25+2*I25</f>
+        <f t="shared" si="1"/>
         <v>290.25</v>
       </c>
       <c r="L25" t="s">
@@ -2189,11 +2453,11 @@
         <v>11.5</v>
       </c>
       <c r="J26">
-        <f>AVERAGE(D26:I26)</f>
+        <f t="shared" si="0"/>
         <v>14.333333333333334</v>
       </c>
       <c r="K26">
-        <f>5*D26 +4.5*E26 +3*F26+3*G26+2.5*H26+2*I26</f>
+        <f t="shared" si="1"/>
         <v>289.5</v>
       </c>
       <c r="L26" t="s">
@@ -2229,11 +2493,11 @@
         <v>13</v>
       </c>
       <c r="J27">
-        <f>AVERAGE(D27:I27)</f>
+        <f t="shared" si="0"/>
         <v>14.208333333333334</v>
       </c>
       <c r="K27">
-        <f>5*D27 +4.5*E27 +3*F27+3*G27+2.5*H27+2*I27</f>
+        <f t="shared" si="1"/>
         <v>288.125</v>
       </c>
       <c r="L27" t="s">
@@ -2269,11 +2533,11 @@
         <v>17</v>
       </c>
       <c r="J28">
-        <f>AVERAGE(D28:I28)</f>
+        <f t="shared" si="0"/>
         <v>14.408333333333333</v>
       </c>
       <c r="K28">
-        <f>5*D28 +4.5*E28 +3*F28+3*G28+2.5*H28+2*I28</f>
+        <f t="shared" si="1"/>
         <v>285.75</v>
       </c>
       <c r="L28" t="s">
@@ -2309,11 +2573,11 @@
         <v>14.5</v>
       </c>
       <c r="J29">
-        <f>AVERAGE(D29:I29)</f>
+        <f t="shared" si="0"/>
         <v>13.5</v>
       </c>
       <c r="K29">
-        <f>5*D29 +4.5*E29 +3*F29+3*G29+2.5*H29+2*I29</f>
+        <f t="shared" si="1"/>
         <v>284.25</v>
       </c>
       <c r="L29" t="s">
@@ -2349,11 +2613,11 @@
         <v>11.25</v>
       </c>
       <c r="J30">
-        <f>AVERAGE(D30:I30)</f>
+        <f t="shared" si="0"/>
         <v>13.791666666666666</v>
       </c>
       <c r="K30">
-        <f>5*D30 +4.5*E30 +3*F30+3*G30+2.5*H30+2*I30</f>
+        <f t="shared" si="1"/>
         <v>284.25</v>
       </c>
       <c r="L30" t="s">
@@ -2389,11 +2653,11 @@
         <v>18</v>
       </c>
       <c r="J31">
-        <f>AVERAGE(D31:I31)</f>
+        <f t="shared" si="0"/>
         <v>14.416666666666666</v>
       </c>
       <c r="K31">
-        <f>5*D31 +4.5*E31 +3*F31+3*G31+2.5*H31+2*I31</f>
+        <f t="shared" si="1"/>
         <v>277.25</v>
       </c>
       <c r="L31" t="s">
@@ -2429,11 +2693,11 @@
         <v>10</v>
       </c>
       <c r="J32">
-        <f>AVERAGE(D32:I32)</f>
+        <f t="shared" si="0"/>
         <v>13.733333333333334</v>
       </c>
       <c r="K32">
-        <f>5*D32 +4.5*E32 +3*F32+3*G32+2.5*H32+2*I32</f>
+        <f t="shared" si="1"/>
         <v>273.57499999999999</v>
       </c>
       <c r="L32" t="s">
@@ -2469,11 +2733,11 @@
         <v>18.5</v>
       </c>
       <c r="J33">
-        <f>AVERAGE(D33:I33)</f>
+        <f t="shared" si="0"/>
         <v>13.958333333333334</v>
       </c>
       <c r="K33">
-        <f>5*D33 +4.5*E33 +3*F33+3*G33+2.5*H33+2*I33</f>
+        <f t="shared" si="1"/>
         <v>273</v>
       </c>
       <c r="L33" t="s">
@@ -2509,11 +2773,11 @@
         <v>14</v>
       </c>
       <c r="J34">
-        <f>AVERAGE(D34:I34)</f>
+        <f t="shared" ref="J34:J52" si="2">AVERAGE(D34:I34)</f>
         <v>13.166666666666666</v>
       </c>
       <c r="K34">
-        <f>5*D34 +4.5*E34 +3*F34+3*G34+2.5*H34+2*I34</f>
+        <f t="shared" ref="K34:K52" si="3">5*D34 +4.5*E34 +3*F34+3*G34+2.5*H34+2*I34</f>
         <v>270.5</v>
       </c>
       <c r="L34" t="s">
@@ -2549,11 +2813,11 @@
         <v>15</v>
       </c>
       <c r="J35">
-        <f>AVERAGE(D35:I35)</f>
+        <f t="shared" si="2"/>
         <v>14.041666666666666</v>
       </c>
       <c r="K35">
-        <f>5*D35 +4.5*E35 +3*F35+3*G35+2.5*H35+2*I35</f>
+        <f t="shared" si="3"/>
         <v>269.25</v>
       </c>
       <c r="L35" t="s">
@@ -2589,11 +2853,11 @@
         <v>10</v>
       </c>
       <c r="J36">
-        <f>AVERAGE(D36:I36)</f>
+        <f t="shared" si="2"/>
         <v>12.366666666666667</v>
       </c>
       <c r="K36">
-        <f>5*D36 +4.5*E36 +3*F36+3*G36+2.5*H36+2*I36</f>
+        <f t="shared" si="3"/>
         <v>267.39999999999998</v>
       </c>
       <c r="L36" t="s">
@@ -2629,11 +2893,11 @@
         <v>15.8</v>
       </c>
       <c r="J37">
-        <f>AVERAGE(D37:I37)</f>
+        <f t="shared" si="2"/>
         <v>13.508333333333333</v>
       </c>
       <c r="K37">
-        <f>5*D37 +4.5*E37 +3*F37+3*G37+2.5*H37+2*I37</f>
+        <f t="shared" si="3"/>
         <v>267.10000000000002</v>
       </c>
       <c r="L37" t="s">
@@ -2669,11 +2933,11 @@
         <v>17</v>
       </c>
       <c r="J38">
-        <f>AVERAGE(D38:I38)</f>
+        <f t="shared" si="2"/>
         <v>13.333333333333334</v>
       </c>
       <c r="K38">
-        <f>5*D38 +4.5*E38 +3*F38+3*G38+2.5*H38+2*I38</f>
+        <f t="shared" si="3"/>
         <v>266</v>
       </c>
       <c r="L38" t="s">
@@ -2709,11 +2973,11 @@
         <v>14.5</v>
       </c>
       <c r="J39">
-        <f>AVERAGE(D39:I39)</f>
+        <f t="shared" si="2"/>
         <v>13.291666666666666</v>
       </c>
       <c r="K39">
-        <f>5*D39 +4.5*E39 +3*F39+3*G39+2.5*H39+2*I39</f>
+        <f t="shared" si="3"/>
         <v>262</v>
       </c>
       <c r="L39" t="s">
@@ -2749,11 +3013,11 @@
         <v>13</v>
       </c>
       <c r="J40">
-        <f>AVERAGE(D40:I40)</f>
+        <f t="shared" si="2"/>
         <v>12.875</v>
       </c>
       <c r="K40">
-        <f>5*D40 +4.5*E40 +3*F40+3*G40+2.5*H40+2*I40</f>
+        <f t="shared" si="3"/>
         <v>260.625</v>
       </c>
       <c r="L40" t="s">
@@ -2789,11 +3053,11 @@
         <v>15.75</v>
       </c>
       <c r="J41">
-        <f>AVERAGE(D41:I41)</f>
+        <f t="shared" si="2"/>
         <v>13.166666666666666</v>
       </c>
       <c r="K41">
-        <f>5*D41 +4.5*E41 +3*F41+3*G41+2.5*H41+2*I41</f>
+        <f t="shared" si="3"/>
         <v>251.875</v>
       </c>
       <c r="L41" t="s">
@@ -2829,11 +3093,11 @@
         <v>10</v>
       </c>
       <c r="J42">
-        <f>AVERAGE(D42:I42)</f>
+        <f t="shared" si="2"/>
         <v>12.408333333333333</v>
       </c>
       <c r="K42">
-        <f>5*D42 +4.5*E42 +3*F42+3*G42+2.5*H42+2*I42</f>
+        <f t="shared" si="3"/>
         <v>251.47499999999999</v>
       </c>
       <c r="L42" t="s">
@@ -2869,11 +3133,11 @@
         <v>12</v>
       </c>
       <c r="J43">
-        <f>AVERAGE(D43:I43)</f>
+        <f t="shared" si="2"/>
         <v>12.125</v>
       </c>
       <c r="K43">
-        <f>5*D43 +4.5*E43 +3*F43+3*G43+2.5*H43+2*I43</f>
+        <f t="shared" si="3"/>
         <v>249.25</v>
       </c>
       <c r="L43" t="s">
@@ -2909,11 +3173,11 @@
         <v>17.5</v>
       </c>
       <c r="J44">
-        <f>AVERAGE(D44:I44)</f>
+        <f t="shared" si="2"/>
         <v>12.458333333333334</v>
       </c>
       <c r="K44">
-        <f>5*D44 +4.5*E44 +3*F44+3*G44+2.5*H44+2*I44</f>
+        <f t="shared" si="3"/>
         <v>242</v>
       </c>
       <c r="L44" t="s">
@@ -2949,11 +3213,11 @@
         <v>10</v>
       </c>
       <c r="J45">
-        <f>AVERAGE(D45:I45)</f>
+        <f t="shared" si="2"/>
         <v>12.033333333333333</v>
       </c>
       <c r="K45">
-        <f>5*D45 +4.5*E45 +3*F45+3*G45+2.5*H45+2*I45</f>
+        <f t="shared" si="3"/>
         <v>238.5</v>
       </c>
       <c r="L45" t="s">
@@ -2989,11 +3253,11 @@
         <v>15</v>
       </c>
       <c r="J46">
-        <f>AVERAGE(D46:I46)</f>
+        <f t="shared" si="2"/>
         <v>11.958333333333334</v>
       </c>
       <c r="K46">
-        <f>5*D46 +4.5*E46 +3*F46+3*G46+2.5*H46+2*I46</f>
+        <f t="shared" si="3"/>
         <v>237.875</v>
       </c>
       <c r="L46" t="s">
@@ -3029,11 +3293,11 @@
         <v>15</v>
       </c>
       <c r="J47">
-        <f>AVERAGE(D47:I47)</f>
+        <f t="shared" si="2"/>
         <v>11.808333333333332</v>
       </c>
       <c r="K47">
-        <f>5*D47 +4.5*E47 +3*F47+3*G47+2.5*H47+2*I47</f>
+        <f t="shared" si="3"/>
         <v>233.65</v>
       </c>
       <c r="L47" t="s">
@@ -3069,11 +3333,11 @@
         <v>16</v>
       </c>
       <c r="J48">
-        <f>AVERAGE(D48:I48)</f>
+        <f t="shared" si="2"/>
         <v>12.049999999999999</v>
       </c>
       <c r="K48">
-        <f>5*D48 +4.5*E48 +3*F48+3*G48+2.5*H48+2*I48</f>
+        <f t="shared" si="3"/>
         <v>231.4</v>
       </c>
       <c r="L48" t="s">
@@ -3109,11 +3373,11 @@
         <v>14</v>
       </c>
       <c r="J49">
-        <f>AVERAGE(D49:I49)</f>
+        <f t="shared" si="2"/>
         <v>11.924999999999999</v>
       </c>
       <c r="K49">
-        <f>5*D49 +4.5*E49 +3*F49+3*G49+2.5*H49+2*I49</f>
+        <f t="shared" si="3"/>
         <v>230.5</v>
       </c>
       <c r="L49" t="s">
@@ -3149,11 +3413,11 @@
         <v>12.25</v>
       </c>
       <c r="J50">
-        <f>AVERAGE(D50:I50)</f>
+        <f t="shared" si="2"/>
         <v>11.458333333333334</v>
       </c>
       <c r="K50">
-        <f>5*D50 +4.5*E50 +3*F50+3*G50+2.5*H50+2*I50</f>
+        <f t="shared" si="3"/>
         <v>229.875</v>
       </c>
       <c r="L50" t="s">
@@ -3189,11 +3453,11 @@
         <v>14</v>
       </c>
       <c r="J51">
-        <f>AVERAGE(D51:I51)</f>
+        <f t="shared" si="2"/>
         <v>11.166666666666666</v>
       </c>
       <c r="K51">
-        <f>5*D51 +4.5*E51 +3*F51+3*G51+2.5*H51+2*I51</f>
+        <f t="shared" si="3"/>
         <v>217</v>
       </c>
       <c r="L51" t="s">
@@ -3229,11 +3493,11 @@
         <v>15.5</v>
       </c>
       <c r="J52">
-        <f>AVERAGE(D52:I52)</f>
+        <f t="shared" si="2"/>
         <v>11.125</v>
       </c>
       <c r="K52">
-        <f>5*D52 +4.5*E52 +3*F52+3*G52+2.5*H52+2*I52</f>
+        <f t="shared" si="3"/>
         <v>214.875</v>
       </c>
       <c r="L52" t="s">
@@ -3253,22 +3517,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F31508D-2E6B-414C-84FF-04448104EB06}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0204A13-5737-4B98-92B5-CE580470D2AF}">
   <dimension ref="A1:M51"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="G1" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K1" sqref="K1:M51"/>
     </sheetView>
   </sheetViews>
@@ -3355,11 +3607,11 @@
         <v>16</v>
       </c>
       <c r="K2">
-        <f>AVERAGE(D2:J2)</f>
+        <f t="shared" ref="K2:K17" si="0">AVERAGE(D2:J2)</f>
         <v>13.142857142857142</v>
       </c>
       <c r="L2">
-        <f>4.5*D2+3.5*E2+3*F2+2.5*H2+3*G2+2*I2+1.5*J2</f>
+        <f t="shared" ref="L2:L33" si="1">4.5*D2+3.5*E2+3*F2+2.5*H2+3*G2+2*I2+1.5*J2</f>
         <v>250.25</v>
       </c>
       <c r="M2" t="s">
@@ -3398,11 +3650,11 @@
         <v>11.25</v>
       </c>
       <c r="K3">
-        <f>AVERAGE(D3:J3)</f>
+        <f t="shared" si="0"/>
         <v>12.642857142857142</v>
       </c>
       <c r="L3">
-        <f>4.5*D3+3.5*E3+3*F3+2.5*H3+3*G3+2*I3+1.5*J3</f>
+        <f t="shared" si="1"/>
         <v>261.375</v>
       </c>
       <c r="M3" t="s">
@@ -3441,11 +3693,11 @@
         <v>18</v>
       </c>
       <c r="K4">
-        <f>AVERAGE(D4:J4)</f>
+        <f t="shared" si="0"/>
         <v>15.285714285714286</v>
       </c>
       <c r="L4">
-        <f>4.5*D4+3.5*E4+3*F4+2.5*H4+3*G4+2*I4+1.5*J4</f>
+        <f t="shared" si="1"/>
         <v>301.75</v>
       </c>
       <c r="M4" t="s">
@@ -3484,11 +3736,11 @@
         <v>19</v>
       </c>
       <c r="K5">
-        <f>AVERAGE(D5:J5)</f>
+        <f t="shared" si="0"/>
         <v>14.152857142857142</v>
       </c>
       <c r="L5">
-        <f>4.5*D5+3.5*E5+3*F5+2.5*H5+3*G5+2*I5+1.5*J5</f>
+        <f t="shared" si="1"/>
         <v>265.58500000000004</v>
       </c>
       <c r="M5" t="s">
@@ -3527,11 +3779,11 @@
         <v>17</v>
       </c>
       <c r="K6">
-        <f>AVERAGE(D6:J6)</f>
+        <f t="shared" si="0"/>
         <v>14.535714285714286</v>
       </c>
       <c r="L6">
-        <f>4.5*D6+3.5*E6+3*F6+2.5*H6+3*G6+2*I6+1.5*J6</f>
+        <f t="shared" si="1"/>
         <v>279.875</v>
       </c>
       <c r="M6" t="s">
@@ -3570,11 +3822,11 @@
         <v>18</v>
       </c>
       <c r="K7">
-        <f>AVERAGE(D7:J7)</f>
+        <f t="shared" si="0"/>
         <v>16.821428571428573</v>
       </c>
       <c r="L7">
-        <f>4.5*D7+3.5*E7+3*F7+2.5*H7+3*G7+2*I7+1.5*J7</f>
+        <f t="shared" si="1"/>
         <v>327.5</v>
       </c>
       <c r="M7" t="s">
@@ -3613,11 +3865,11 @@
         <v>18</v>
       </c>
       <c r="K8">
-        <f>AVERAGE(D8:J8)</f>
+        <f t="shared" si="0"/>
         <v>15.707142857142857</v>
       </c>
       <c r="L8">
-        <f>4.5*D8+3.5*E8+3*F8+2.5*H8+3*G8+2*I8+1.5*J8</f>
+        <f t="shared" si="1"/>
         <v>297.82499999999999</v>
       </c>
       <c r="M8" t="s">
@@ -3656,11 +3908,11 @@
         <v>18</v>
       </c>
       <c r="K9">
-        <f>AVERAGE(D9:J9)</f>
+        <f t="shared" si="0"/>
         <v>14.75</v>
       </c>
       <c r="L9">
-        <f>4.5*D9+3.5*E9+3*F9+2.5*H9+3*G9+2*I9+1.5*J9</f>
+        <f t="shared" si="1"/>
         <v>283.625</v>
       </c>
       <c r="M9" t="s">
@@ -3699,11 +3951,11 @@
         <v>18.5</v>
       </c>
       <c r="K10">
-        <f>AVERAGE(D10:J10)</f>
+        <f t="shared" si="0"/>
         <v>14.857142857142858</v>
       </c>
       <c r="L10">
-        <f>4.5*D10+3.5*E10+3*F10+2.5*H10+3*G10+2*I10+1.5*J10</f>
+        <f t="shared" si="1"/>
         <v>282.75</v>
       </c>
       <c r="M10" t="s">
@@ -3742,11 +3994,11 @@
         <v>20</v>
       </c>
       <c r="K11">
-        <f>AVERAGE(D11:J11)</f>
+        <f t="shared" si="0"/>
         <v>14.299999999999999</v>
       </c>
       <c r="L11">
-        <f>4.5*D11+3.5*E11+3*F11+2.5*H11+3*G11+2*I11+1.5*J11</f>
+        <f t="shared" si="1"/>
         <v>267.42500000000001</v>
       </c>
       <c r="M11" t="s">
@@ -3785,11 +4037,11 @@
         <v>19</v>
       </c>
       <c r="K12">
-        <f>AVERAGE(D12:J12)</f>
+        <f t="shared" si="0"/>
         <v>12.714285714285714</v>
       </c>
       <c r="L12">
-        <f>4.5*D12+3.5*E12+3*F12+2.5*H12+3*G12+2*I12+1.5*J12</f>
+        <f t="shared" si="1"/>
         <v>247.875</v>
       </c>
       <c r="M12" t="s">
@@ -3828,11 +4080,11 @@
         <v>17</v>
       </c>
       <c r="K13">
-        <f>AVERAGE(D13:J13)</f>
+        <f t="shared" si="0"/>
         <v>14.928571428571429</v>
       </c>
       <c r="L13">
-        <f>4.5*D13+3.5*E13+3*F13+2.5*H13+3*G13+2*I13+1.5*J13</f>
+        <f t="shared" si="1"/>
         <v>286.375</v>
       </c>
       <c r="M13" t="s">
@@ -3871,11 +4123,11 @@
         <v>13.25</v>
       </c>
       <c r="K14">
-        <f>AVERAGE(D14:J14)</f>
+        <f t="shared" si="0"/>
         <v>12.535714285714286</v>
       </c>
       <c r="L14">
-        <f>4.5*D14+3.5*E14+3*F14+2.5*H14+3*G14+2*I14+1.5*J14</f>
+        <f t="shared" si="1"/>
         <v>247.5</v>
       </c>
       <c r="M14" t="s">
@@ -3914,11 +4166,11 @@
         <v>15.5</v>
       </c>
       <c r="K15">
-        <f>AVERAGE(D15:J15)</f>
+        <f t="shared" si="0"/>
         <v>12.071428571428571</v>
       </c>
       <c r="L15">
-        <f>4.5*D15+3.5*E15+3*F15+2.5*H15+3*G15+2*I15+1.5*J15</f>
+        <f t="shared" si="1"/>
         <v>238.625</v>
       </c>
       <c r="M15" t="s">
@@ -3957,11 +4209,11 @@
         <v>15</v>
       </c>
       <c r="K16">
-        <f>AVERAGE(D16:J16)</f>
+        <f t="shared" si="0"/>
         <v>15.464285714285714</v>
       </c>
       <c r="L16">
-        <f>4.5*D16+3.5*E16+3*F16+2.5*H16+3*G16+2*I16+1.5*J16</f>
+        <f t="shared" si="1"/>
         <v>303.75</v>
       </c>
       <c r="M16" t="s">
@@ -4000,11 +4252,11 @@
         <v>14.25</v>
       </c>
       <c r="K17">
-        <f>AVERAGE(D17:J17)</f>
+        <f t="shared" si="0"/>
         <v>14.678571428571429</v>
       </c>
       <c r="L17">
-        <f>4.5*D17+3.5*E17+3*F17+2.5*H17+3*G17+2*I17+1.5*J17</f>
+        <f t="shared" si="1"/>
         <v>289.75</v>
       </c>
       <c r="M17" t="s">
@@ -4047,7 +4299,7 @@
         <v>14.55</v>
       </c>
       <c r="L18">
-        <f>4.5*D18+3.5*E18+3*F18+2.5*H18+3*G18+2*I18+1.5*J18</f>
+        <f t="shared" si="1"/>
         <v>278.49</v>
       </c>
       <c r="M18" t="s">
@@ -4086,11 +4338,11 @@
         <v>12.25</v>
       </c>
       <c r="K19">
-        <f>AVERAGE(D19:J19)</f>
+        <f t="shared" ref="K19:K51" si="2">AVERAGE(D19:J19)</f>
         <v>13.178571428571429</v>
       </c>
       <c r="L19">
-        <f>4.5*D19+3.5*E19+3*F19+2.5*H19+3*G19+2*I19+1.5*J19</f>
+        <f t="shared" si="1"/>
         <v>271.625</v>
       </c>
       <c r="M19" t="s">
@@ -4129,11 +4381,11 @@
         <v>13.75</v>
       </c>
       <c r="K20">
-        <f>AVERAGE(D20:J20)</f>
+        <f t="shared" si="2"/>
         <v>15.035714285714286</v>
       </c>
       <c r="L20">
-        <f>4.5*D20+3.5*E20+3*F20+2.5*H20+3*G20+2*I20+1.5*J20</f>
+        <f t="shared" si="1"/>
         <v>306.5</v>
       </c>
       <c r="M20" t="s">
@@ -4172,11 +4424,11 @@
         <v>15.75</v>
       </c>
       <c r="K21">
-        <f>AVERAGE(D21:J21)</f>
+        <f t="shared" si="2"/>
         <v>12.821428571428571</v>
       </c>
       <c r="L21">
-        <f>4.5*D21+3.5*E21+3*F21+2.5*H21+3*G21+2*I21+1.5*J21</f>
+        <f t="shared" si="1"/>
         <v>248.75</v>
       </c>
       <c r="M21" t="s">
@@ -4215,11 +4467,11 @@
         <v>14.5</v>
       </c>
       <c r="K22">
-        <f>AVERAGE(D22:J22)</f>
+        <f t="shared" si="2"/>
         <v>13.25</v>
       </c>
       <c r="L22">
-        <f>4.5*D22+3.5*E22+3*F22+2.5*H22+3*G22+2*I22+1.5*J22</f>
+        <f t="shared" si="1"/>
         <v>260</v>
       </c>
       <c r="M22" t="s">
@@ -4258,11 +4510,11 @@
         <v>14.25</v>
       </c>
       <c r="K23">
-        <f>AVERAGE(D23:J23)</f>
+        <f t="shared" si="2"/>
         <v>13.540000000000001</v>
       </c>
       <c r="L23">
-        <f>4.5*D23+3.5*E23+3*F23+2.5*H23+3*G23+2*I23+1.5*J23</f>
+        <f t="shared" si="1"/>
         <v>263.46500000000003</v>
       </c>
       <c r="M23" t="s">
@@ -4301,11 +4553,11 @@
         <v>16</v>
       </c>
       <c r="K24">
-        <f>AVERAGE(D24:J24)</f>
+        <f t="shared" si="2"/>
         <v>14.035714285714286</v>
       </c>
       <c r="L24">
-        <f>4.5*D24+3.5*E24+3*F24+2.5*H24+3*G24+2*I24+1.5*J24</f>
+        <f t="shared" si="1"/>
         <v>280.125</v>
       </c>
       <c r="M24" t="s">
@@ -4344,11 +4596,11 @@
         <v>14</v>
       </c>
       <c r="K25">
-        <f>AVERAGE(D25:J25)</f>
+        <f t="shared" si="2"/>
         <v>15.721428571428572</v>
       </c>
       <c r="L25">
-        <f>4.5*D25+3.5*E25+3*F25+2.5*H25+3*G25+2*I25+1.5*J25</f>
+        <f t="shared" si="1"/>
         <v>310.02499999999998</v>
       </c>
       <c r="M25" t="s">
@@ -4387,11 +4639,11 @@
         <v>17</v>
       </c>
       <c r="K26">
-        <f>AVERAGE(D26:J26)</f>
+        <f t="shared" si="2"/>
         <v>15.928571428571429</v>
       </c>
       <c r="L26">
-        <f>4.5*D26+3.5*E26+3*F26+2.5*H26+3*G26+2*I26+1.5*J26</f>
+        <f t="shared" si="1"/>
         <v>310.625</v>
       </c>
       <c r="M26" t="s">
@@ -4430,11 +4682,11 @@
         <v>15.75</v>
       </c>
       <c r="K27">
-        <f>AVERAGE(D27:J27)</f>
+        <f t="shared" si="2"/>
         <v>13.414285714285715</v>
       </c>
       <c r="L27">
-        <f>4.5*D27+3.5*E27+3*F27+2.5*H27+3*G27+2*I27+1.5*J27</f>
+        <f t="shared" si="1"/>
         <v>258.57499999999999</v>
       </c>
       <c r="M27" t="s">
@@ -4473,11 +4725,11 @@
         <v>16.5</v>
       </c>
       <c r="K28">
-        <f>AVERAGE(D28:J28)</f>
+        <f t="shared" si="2"/>
         <v>14.342857142857143</v>
       </c>
       <c r="L28">
-        <f>4.5*D28+3.5*E28+3*F28+2.5*H28+3*G28+2*I28+1.5*J28</f>
+        <f t="shared" si="1"/>
         <v>276.05</v>
       </c>
       <c r="M28" t="s">
@@ -4516,11 +4768,11 @@
         <v>17.5</v>
       </c>
       <c r="K29">
-        <f>AVERAGE(D29:J29)</f>
+        <f t="shared" si="2"/>
         <v>13.857142857142858</v>
       </c>
       <c r="L29">
-        <f>4.5*D29+3.5*E29+3*F29+2.5*H29+3*G29+2*I29+1.5*J29</f>
+        <f t="shared" si="1"/>
         <v>268.625</v>
       </c>
       <c r="M29" t="s">
@@ -4559,11 +4811,11 @@
         <v>14</v>
       </c>
       <c r="K30">
-        <f>AVERAGE(D30:J30)</f>
+        <f t="shared" si="2"/>
         <v>15.242857142857144</v>
       </c>
       <c r="L30">
-        <f>4.5*D30+3.5*E30+3*F30+2.5*H30+3*G30+2*I30+1.5*J30</f>
+        <f t="shared" si="1"/>
         <v>304.10000000000002</v>
       </c>
       <c r="M30" t="s">
@@ -4602,11 +4854,11 @@
         <v>17.5</v>
       </c>
       <c r="K31">
-        <f>AVERAGE(D31:J31)</f>
+        <f t="shared" si="2"/>
         <v>16.035714285714285</v>
       </c>
       <c r="L31">
-        <f>4.5*D31+3.5*E31+3*F31+2.5*H31+3*G31+2*I31+1.5*J31</f>
+        <f t="shared" si="1"/>
         <v>316.875</v>
       </c>
       <c r="M31" t="s">
@@ -4645,11 +4897,11 @@
         <v>10.25</v>
       </c>
       <c r="K32">
-        <f>AVERAGE(D32:J32)</f>
+        <f t="shared" si="2"/>
         <v>13.857142857142858</v>
       </c>
       <c r="L32">
-        <f>4.5*D32+3.5*E32+3*F32+2.5*H32+3*G32+2*I32+1.5*J32</f>
+        <f t="shared" si="1"/>
         <v>284.75</v>
       </c>
       <c r="M32" t="s">
@@ -4688,11 +4940,11 @@
         <v>11.5</v>
       </c>
       <c r="K33">
-        <f>AVERAGE(D33:J33)</f>
+        <f t="shared" si="2"/>
         <v>13.742857142857144</v>
       </c>
       <c r="L33">
-        <f>4.5*D33+3.5*E33+3*F33+2.5*H33+3*G33+2*I33+1.5*J33</f>
+        <f t="shared" si="1"/>
         <v>284.27499999999998</v>
       </c>
       <c r="M33" t="s">
@@ -4731,11 +4983,11 @@
         <v>11.5</v>
       </c>
       <c r="K34">
-        <f>AVERAGE(D34:J34)</f>
+        <f t="shared" si="2"/>
         <v>13.107142857142858</v>
       </c>
       <c r="L34">
-        <f>4.5*D34+3.5*E34+3*F34+2.5*H34+3*G34+2*I34+1.5*J34</f>
+        <f t="shared" ref="L34:L51" si="3">4.5*D34+3.5*E34+3*F34+2.5*H34+3*G34+2*I34+1.5*J34</f>
         <v>268.375</v>
       </c>
       <c r="M34" t="s">
@@ -4774,11 +5026,11 @@
         <v>17</v>
       </c>
       <c r="K35">
-        <f>AVERAGE(D35:J35)</f>
+        <f t="shared" si="2"/>
         <v>14.607142857142858</v>
       </c>
       <c r="L35">
-        <f>4.5*D35+3.5*E35+3*F35+2.5*H35+3*G35+2*I35+1.5*J35</f>
+        <f t="shared" si="3"/>
         <v>289.5</v>
       </c>
       <c r="M35" t="s">
@@ -4817,11 +5069,11 @@
         <v>14.25</v>
       </c>
       <c r="K36">
-        <f>AVERAGE(D36:J36)</f>
+        <f t="shared" si="2"/>
         <v>12.907142857142857</v>
       </c>
       <c r="L36">
-        <f>4.5*D36+3.5*E36+3*F36+2.5*H36+3*G36+2*I36+1.5*J36</f>
+        <f t="shared" si="3"/>
         <v>261.2</v>
       </c>
       <c r="M36" t="s">
@@ -4860,11 +5112,11 @@
         <v>18</v>
       </c>
       <c r="K37">
-        <f>AVERAGE(D37:J37)</f>
+        <f t="shared" si="2"/>
         <v>14.785714285714286</v>
       </c>
       <c r="L37">
-        <f>4.5*D37+3.5*E37+3*F37+2.5*H37+3*G37+2*I37+1.5*J37</f>
+        <f t="shared" si="3"/>
         <v>295.625</v>
       </c>
       <c r="M37" t="s">
@@ -4903,11 +5155,11 @@
         <v>20</v>
       </c>
       <c r="K38">
-        <f>AVERAGE(D38:J38)</f>
+        <f t="shared" si="2"/>
         <v>16.178571428571427</v>
       </c>
       <c r="L38">
-        <f>4.5*D38+3.5*E38+3*F38+2.5*H38+3*G38+2*I38+1.5*J38</f>
+        <f t="shared" si="3"/>
         <v>314.75</v>
       </c>
       <c r="M38" t="s">
@@ -4946,11 +5198,11 @@
         <v>17</v>
       </c>
       <c r="K39">
-        <f>AVERAGE(D39:J39)</f>
+        <f t="shared" si="2"/>
         <v>15.142857142857142</v>
       </c>
       <c r="L39">
-        <f>4.5*D39+3.5*E39+3*F39+2.5*H39+3*G39+2*I39+1.5*J39</f>
+        <f t="shared" si="3"/>
         <v>293.875</v>
       </c>
       <c r="M39" t="s">
@@ -4989,11 +5241,11 @@
         <v>11.5</v>
       </c>
       <c r="K40">
-        <f>AVERAGE(D40:J40)</f>
+        <f t="shared" si="2"/>
         <v>11.857142857142858</v>
       </c>
       <c r="L40">
-        <f>4.5*D40+3.5*E40+3*F40+2.5*H40+3*G40+2*I40+1.5*J40</f>
+        <f t="shared" si="3"/>
         <v>234.625</v>
       </c>
       <c r="M40" t="s">
@@ -5032,11 +5284,11 @@
         <v>16</v>
       </c>
       <c r="K41">
-        <f>AVERAGE(D41:J41)</f>
+        <f t="shared" si="2"/>
         <v>14.914285714285715</v>
       </c>
       <c r="L41">
-        <f>4.5*D41+3.5*E41+3*F41+2.5*H41+3*G41+2*I41+1.5*J41</f>
+        <f t="shared" si="3"/>
         <v>285.07499999999999</v>
       </c>
       <c r="M41" t="s">
@@ -5075,11 +5327,11 @@
         <v>14</v>
       </c>
       <c r="K42">
-        <f>AVERAGE(D42:J42)</f>
+        <f t="shared" si="2"/>
         <v>13.892857142857142</v>
       </c>
       <c r="L42">
-        <f>4.5*D42+3.5*E42+3*F42+2.5*H42+3*G42+2*I42+1.5*J42</f>
+        <f t="shared" si="3"/>
         <v>271.125</v>
       </c>
       <c r="M42" t="s">
@@ -5118,11 +5370,11 @@
         <v>13</v>
       </c>
       <c r="K43">
-        <f>AVERAGE(D43:J43)</f>
+        <f t="shared" si="2"/>
         <v>15.178571428571429</v>
       </c>
       <c r="L43">
-        <f>4.5*D43+3.5*E43+3*F43+2.5*H43+3*G43+2*I43+1.5*J43</f>
+        <f t="shared" si="3"/>
         <v>292.125</v>
       </c>
       <c r="M43" t="s">
@@ -5161,11 +5413,11 @@
         <v>12</v>
       </c>
       <c r="K44">
-        <f>AVERAGE(D44:J44)</f>
+        <f t="shared" si="2"/>
         <v>11.942857142857141</v>
       </c>
       <c r="L44">
-        <f>4.5*D44+3.5*E44+3*F44+2.5*H44+3*G44+2*I44+1.5*J44</f>
+        <f t="shared" si="3"/>
         <v>237.8</v>
       </c>
       <c r="M44" t="s">
@@ -5204,11 +5456,11 @@
         <v>12.5</v>
       </c>
       <c r="K45">
-        <f>AVERAGE(D45:J45)</f>
+        <f t="shared" si="2"/>
         <v>13.75</v>
       </c>
       <c r="L45">
-        <f>4.5*D45+3.5*E45+3*F45+2.5*H45+3*G45+2*I45+1.5*J45</f>
+        <f t="shared" si="3"/>
         <v>277.125</v>
       </c>
       <c r="M45" t="s">
@@ -5247,11 +5499,11 @@
         <v>19</v>
       </c>
       <c r="K46">
-        <f>AVERAGE(D46:J46)</f>
+        <f t="shared" si="2"/>
         <v>14.178571428571429</v>
       </c>
       <c r="L46">
-        <f>4.5*D46+3.5*E46+3*F46+2.5*H46+3*G46+2*I46+1.5*J46</f>
+        <f t="shared" si="3"/>
         <v>271.5</v>
       </c>
       <c r="M46" t="s">
@@ -5290,11 +5542,11 @@
         <v>18</v>
       </c>
       <c r="K47">
-        <f>AVERAGE(D47:J47)</f>
+        <f t="shared" si="2"/>
         <v>15.821428571428571</v>
       </c>
       <c r="L47">
-        <f>4.5*D47+3.5*E47+3*F47+2.5*H47+3*G47+2*I47+1.5*J47</f>
+        <f t="shared" si="3"/>
         <v>311.875</v>
       </c>
       <c r="M47" t="s">
@@ -5333,11 +5585,11 @@
         <v>15</v>
       </c>
       <c r="K48">
-        <f>AVERAGE(D48:J48)</f>
+        <f t="shared" si="2"/>
         <v>13.928571428571429</v>
       </c>
       <c r="L48">
-        <f>4.5*D48+3.5*E48+3*F48+2.5*H48+3*G48+2*I48+1.5*J48</f>
+        <f t="shared" si="3"/>
         <v>266</v>
       </c>
       <c r="M48" t="s">
@@ -5376,11 +5628,11 @@
         <v>13</v>
       </c>
       <c r="K49">
-        <f>AVERAGE(D49:J49)</f>
+        <f t="shared" si="2"/>
         <v>12.785714285714286</v>
       </c>
       <c r="L49">
-        <f>4.5*D49+3.5*E49+3*F49+2.5*H49+3*G49+2*I49+1.5*J49</f>
+        <f t="shared" si="3"/>
         <v>257.75</v>
       </c>
       <c r="M49" t="s">
@@ -5419,11 +5671,11 @@
         <v>12</v>
       </c>
       <c r="K50">
-        <f>AVERAGE(D50:J50)</f>
+        <f t="shared" si="2"/>
         <v>14.357142857142858</v>
       </c>
       <c r="L50">
-        <f>4.5*D50+3.5*E50+3*F50+2.5*H50+3*G50+2*I50+1.5*J50</f>
+        <f t="shared" si="3"/>
         <v>285.875</v>
       </c>
       <c r="M50" t="s">
@@ -5462,11 +5714,11 @@
         <v>15.5</v>
       </c>
       <c r="K51">
-        <f>AVERAGE(D51:J51)</f>
+        <f t="shared" si="2"/>
         <v>15.328571428571427</v>
       </c>
       <c r="L51">
-        <f>4.5*D51+3.5*E51+3*F51+2.5*H51+3*G51+2*I51+1.5*J51</f>
+        <f t="shared" si="3"/>
         <v>305.22500000000002</v>
       </c>
       <c r="M51" t="s">
@@ -5481,7 +5733,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0839CE46-99D2-43C0-A8B1-A621F9C37465}">
   <dimension ref="A1:H102"/>
   <sheetViews>
@@ -8156,12 +8408,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F0A1526-08CC-4229-B633-0A9B05A1F5CF}">
   <dimension ref="A1:F52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="F1" sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8171,60 +8423,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="15" t="s">
         <v>173</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="15" t="s">
         <v>181</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="15" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>10000050</v>
+        <v>10000029</v>
       </c>
       <c r="B2" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="C2" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="D2">
-        <v>15.041666666666666</v>
+        <v>19.041666666666668</v>
       </c>
       <c r="E2">
-        <v>303.25</v>
+        <v>378.875</v>
       </c>
       <c r="F2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>10000049</v>
+        <v>10000038</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D3">
-        <v>15.625</v>
+        <v>18.458333333333332</v>
       </c>
       <c r="E3">
-        <v>315.5</v>
+        <v>367.375</v>
       </c>
       <c r="F3" t="s">
         <v>187</v>
@@ -8232,19 +8484,19 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>10000048</v>
+        <v>10000017</v>
       </c>
       <c r="B4" t="s">
-        <v>84</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>65</v>
+        <v>38</v>
       </c>
       <c r="D4">
-        <v>17.375</v>
+        <v>17.75</v>
       </c>
       <c r="E4">
-        <v>345.5</v>
+        <v>358.75</v>
       </c>
       <c r="F4" t="s">
         <v>187</v>
@@ -8252,79 +8504,79 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>10000047</v>
+        <v>10000031</v>
       </c>
       <c r="B5" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="C5" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="D5">
-        <v>13.958333333333334</v>
+        <v>17.383333333333333</v>
       </c>
       <c r="E5">
-        <v>273</v>
+        <v>346.25</v>
       </c>
       <c r="F5" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>10000046</v>
+        <v>10000048</v>
       </c>
       <c r="B6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D6">
-        <v>14.958333333333334</v>
+        <v>17.375</v>
       </c>
       <c r="E6">
-        <v>303.625</v>
+        <v>345.5</v>
       </c>
       <c r="F6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>10000045</v>
+        <v>10000035</v>
       </c>
       <c r="B7" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="C7" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="D7">
-        <v>13.791666666666666</v>
+        <v>16.400000000000002</v>
       </c>
       <c r="E7">
-        <v>284.25</v>
+        <v>321.375</v>
       </c>
       <c r="F7" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>10000044</v>
+        <v>10000013</v>
       </c>
       <c r="B8" t="s">
-        <v>82</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>61</v>
+        <v>35</v>
       </c>
       <c r="D8">
-        <v>15.833333333333334</v>
+        <v>15.875</v>
       </c>
       <c r="E8">
-        <v>312</v>
+        <v>321</v>
       </c>
       <c r="F8" t="s">
         <v>187</v>
@@ -8332,99 +8584,99 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>10000043</v>
+        <v>10000008</v>
       </c>
       <c r="B9" t="s">
-        <v>81</v>
+        <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="D9">
-        <v>11.958333333333334</v>
+        <v>15.833333333333334</v>
       </c>
       <c r="E9">
-        <v>237.875</v>
+        <v>320.25</v>
       </c>
       <c r="F9" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>10000042</v>
+        <v>10000028</v>
       </c>
       <c r="B10" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="C10" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="D10">
-        <v>12.049999999999999</v>
+        <v>15.591666666666667</v>
       </c>
       <c r="E10">
-        <v>231.4</v>
+        <v>318.85000000000002</v>
       </c>
       <c r="F10" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>10000041</v>
+        <v>10000049</v>
       </c>
       <c r="B11" t="s">
-        <v>79</v>
+        <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D11">
-        <v>11.125</v>
+        <v>15.625</v>
       </c>
       <c r="E11">
-        <v>214.875</v>
+        <v>315.5</v>
       </c>
       <c r="F11" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>10000040</v>
+        <v>10000044</v>
       </c>
       <c r="B12" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="C12" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="D12">
-        <v>13.333333333333334</v>
+        <v>15.833333333333334</v>
       </c>
       <c r="E12">
-        <v>266</v>
+        <v>312</v>
       </c>
       <c r="F12" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>10000039</v>
+        <v>10000030</v>
       </c>
       <c r="B13" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C13" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="D13">
-        <v>14.625</v>
+        <v>15.333333333333334</v>
       </c>
       <c r="E13">
-        <v>292.5</v>
+        <v>309.25</v>
       </c>
       <c r="F13" t="s">
         <v>188</v>
@@ -8432,19 +8684,19 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>10000038</v>
+        <v>10000032</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D14">
-        <v>18.458333333333332</v>
+        <v>15.566666666666668</v>
       </c>
       <c r="E14">
-        <v>367.375</v>
+        <v>304.92500000000001</v>
       </c>
       <c r="F14" t="s">
         <v>187</v>
@@ -8452,79 +8704,79 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>10000037</v>
+        <v>10000046</v>
       </c>
       <c r="B15" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="C15" t="s">
-        <v>22</v>
+        <v>63</v>
       </c>
       <c r="D15">
-        <v>11.808333333333332</v>
+        <v>14.958333333333334</v>
       </c>
       <c r="E15">
-        <v>233.65</v>
+        <v>303.625</v>
       </c>
       <c r="F15" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>10000036</v>
+        <v>10000050</v>
       </c>
       <c r="B16" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="C16" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="D16">
-        <v>11.458333333333334</v>
+        <v>15.041666666666666</v>
       </c>
       <c r="E16">
-        <v>229.875</v>
+        <v>303.25</v>
       </c>
       <c r="F16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>10000035</v>
+        <v>10000018</v>
       </c>
       <c r="B17" t="s">
-        <v>74</v>
+        <v>20</v>
       </c>
       <c r="C17" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="D17">
-        <v>16.400000000000002</v>
+        <v>15.833333333333334</v>
       </c>
       <c r="E17">
-        <v>321.375</v>
+        <v>301.75</v>
       </c>
       <c r="F17" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>10000034</v>
+        <v>10000009</v>
       </c>
       <c r="B18" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C18" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="D18">
-        <v>14.408333333333333</v>
+        <v>14.708333333333334</v>
       </c>
       <c r="E18">
-        <v>285.75</v>
+        <v>300.75</v>
       </c>
       <c r="F18" t="s">
         <v>188</v>
@@ -8532,79 +8784,79 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>10000033</v>
+        <v>10000015</v>
       </c>
       <c r="B19" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="D19">
-        <v>13.166666666666666</v>
+        <v>15.25</v>
       </c>
       <c r="E19">
-        <v>270.5</v>
+        <v>299.75</v>
       </c>
       <c r="F19" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>10000032</v>
+        <v>10000025</v>
       </c>
       <c r="B20" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="C20" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="D20">
-        <v>15.566666666666668</v>
+        <v>14.094999999999999</v>
       </c>
       <c r="E20">
-        <v>304.92500000000001</v>
+        <v>297.47500000000002</v>
       </c>
       <c r="F20" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>10000031</v>
+        <v>10000022</v>
       </c>
       <c r="B21" t="s">
-        <v>73</v>
+        <v>16</v>
       </c>
       <c r="C21" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="D21">
-        <v>17.383333333333333</v>
+        <v>14.258333333333333</v>
       </c>
       <c r="E21">
-        <v>346.25</v>
+        <v>296.97500000000002</v>
       </c>
       <c r="F21" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>10000030</v>
+        <v>10000006</v>
       </c>
       <c r="B22" t="s">
-        <v>72</v>
+        <v>9</v>
       </c>
       <c r="C22" t="s">
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="D22">
-        <v>15.333333333333334</v>
+        <v>14.878333333333332</v>
       </c>
       <c r="E22">
-        <v>309.25</v>
+        <v>294.81</v>
       </c>
       <c r="F22" t="s">
         <v>188</v>
@@ -8612,159 +8864,159 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>10000029</v>
+        <v>10000023</v>
       </c>
       <c r="B23" t="s">
-        <v>71</v>
+        <v>7</v>
       </c>
       <c r="C23" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D23">
-        <v>19.041666666666668</v>
+        <v>15.125</v>
       </c>
       <c r="E23">
-        <v>378.875</v>
+        <v>294.375</v>
       </c>
       <c r="F23" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>10000028</v>
+        <v>10000039</v>
       </c>
       <c r="B24" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="C24" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="D24">
-        <v>15.591666666666667</v>
+        <v>14.625</v>
       </c>
       <c r="E24">
-        <v>318.85000000000002</v>
+        <v>292.5</v>
       </c>
       <c r="F24" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25">
-        <v>10000027</v>
+        <v>10000010</v>
       </c>
       <c r="B25" t="s">
-        <v>69</v>
+        <v>13</v>
       </c>
       <c r="C25" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="D25">
-        <v>12.033333333333333</v>
+        <v>14.583333333333334</v>
       </c>
       <c r="E25">
-        <v>238.5</v>
+        <v>290.25</v>
       </c>
       <c r="F25" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26">
-        <v>10000026</v>
+        <v>10000011</v>
       </c>
       <c r="B26" t="s">
-        <v>68</v>
+        <v>14</v>
       </c>
       <c r="C26" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="D26">
-        <v>13.166666666666666</v>
+        <v>14.333333333333334</v>
       </c>
       <c r="E26">
-        <v>251.875</v>
+        <v>289.5</v>
       </c>
       <c r="F26" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27">
-        <v>10000025</v>
+        <v>10000001</v>
       </c>
       <c r="B27" t="s">
-        <v>67</v>
+        <v>4</v>
       </c>
       <c r="C27" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="D27">
-        <v>14.094999999999999</v>
+        <v>14.208333333333334</v>
       </c>
       <c r="E27">
-        <v>297.47500000000002</v>
+        <v>288.125</v>
       </c>
       <c r="F27" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28">
-        <v>10000024</v>
+        <v>10000034</v>
       </c>
       <c r="B28" t="s">
-        <v>66</v>
+        <v>10</v>
       </c>
       <c r="C28" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="D28">
-        <v>12.125</v>
+        <v>14.408333333333333</v>
       </c>
       <c r="E28">
-        <v>249.25</v>
+        <v>285.75</v>
       </c>
       <c r="F28" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29">
-        <v>10000023</v>
+        <v>10000045</v>
       </c>
       <c r="B29" t="s">
-        <v>7</v>
+        <v>83</v>
       </c>
       <c r="C29" t="s">
-        <v>41</v>
+        <v>62</v>
       </c>
       <c r="D29">
-        <v>15.125</v>
+        <v>13.791666666666666</v>
       </c>
       <c r="E29">
-        <v>294.375</v>
+        <v>284.25</v>
       </c>
       <c r="F29" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30">
-        <v>10000022</v>
+        <v>10000020</v>
       </c>
       <c r="B30" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="C30" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="D30">
-        <v>14.258333333333333</v>
+        <v>13.5</v>
       </c>
       <c r="E30">
-        <v>296.97500000000002</v>
+        <v>284.25</v>
       </c>
       <c r="F30" t="s">
         <v>189</v>
@@ -8772,39 +9024,39 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31">
-        <v>10000021</v>
+        <v>10000016</v>
       </c>
       <c r="B31" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C31" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D31">
-        <v>13.508333333333333</v>
+        <v>14.416666666666666</v>
       </c>
       <c r="E31">
-        <v>267.10000000000002</v>
+        <v>277.25</v>
       </c>
       <c r="F31" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32">
-        <v>10000020</v>
+        <v>10000007</v>
       </c>
       <c r="B32" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C32" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D32">
-        <v>13.5</v>
+        <v>13.733333333333334</v>
       </c>
       <c r="E32">
-        <v>284.25</v>
+        <v>273.57499999999999</v>
       </c>
       <c r="F32" t="s">
         <v>189</v>
@@ -8812,119 +9064,119 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33">
-        <v>10000019</v>
+        <v>10000047</v>
       </c>
       <c r="B33" t="s">
-        <v>21</v>
+        <v>85</v>
       </c>
       <c r="C33" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="D33">
-        <v>12.458333333333334</v>
+        <v>13.958333333333334</v>
       </c>
       <c r="E33">
-        <v>242</v>
+        <v>273</v>
       </c>
       <c r="F33" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34">
-        <v>10000018</v>
+        <v>10000033</v>
       </c>
       <c r="B34" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="C34" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="D34">
-        <v>15.833333333333334</v>
+        <v>13.166666666666666</v>
       </c>
       <c r="E34">
-        <v>301.75</v>
+        <v>270.5</v>
       </c>
       <c r="F34" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35">
-        <v>10000017</v>
+        <v>10000005</v>
       </c>
       <c r="B35" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="C35" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="D35">
-        <v>17.75</v>
+        <v>14.041666666666666</v>
       </c>
       <c r="E35">
-        <v>358.75</v>
+        <v>269.25</v>
       </c>
       <c r="F35" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36">
-        <v>10000016</v>
+        <v>10000004</v>
       </c>
       <c r="B36" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C36" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="D36">
-        <v>14.416666666666666</v>
+        <v>12.366666666666667</v>
       </c>
       <c r="E36">
-        <v>277.25</v>
+        <v>267.39999999999998</v>
       </c>
       <c r="F36" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37">
-        <v>10000015</v>
+        <v>10000021</v>
       </c>
       <c r="B37" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C37" t="s">
         <v>34</v>
       </c>
       <c r="D37">
-        <v>15.25</v>
+        <v>13.508333333333333</v>
       </c>
       <c r="E37">
-        <v>299.75</v>
+        <v>267.10000000000002</v>
       </c>
       <c r="F37" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38">
-        <v>10000014</v>
+        <v>10000040</v>
       </c>
       <c r="B38" t="s">
-        <v>4</v>
+        <v>78</v>
       </c>
       <c r="C38" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="D38">
-        <v>13.291666666666666</v>
+        <v>13.333333333333334</v>
       </c>
       <c r="E38">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="F38" t="s">
         <v>189</v>
@@ -8932,199 +9184,199 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39">
-        <v>10000013</v>
+        <v>10000014</v>
       </c>
       <c r="B39" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="C39" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D39">
-        <v>15.875</v>
+        <v>13.291666666666666</v>
       </c>
       <c r="E39">
-        <v>321</v>
+        <v>262</v>
       </c>
       <c r="F39" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40">
-        <v>10000012</v>
+        <v>10000002</v>
       </c>
       <c r="B40" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C40" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="D40">
-        <v>12.408333333333333</v>
+        <v>12.875</v>
       </c>
       <c r="E40">
-        <v>251.47499999999999</v>
+        <v>260.625</v>
       </c>
       <c r="F40" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41">
-        <v>10000011</v>
+        <v>10000026</v>
       </c>
       <c r="B41" t="s">
-        <v>14</v>
+        <v>68</v>
       </c>
       <c r="C41" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="D41">
-        <v>14.333333333333334</v>
+        <v>13.166666666666666</v>
       </c>
       <c r="E41">
-        <v>289.5</v>
+        <v>251.875</v>
       </c>
       <c r="F41" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42">
-        <v>10000010</v>
+        <v>10000012</v>
       </c>
       <c r="B42" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C42" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D42">
-        <v>14.583333333333334</v>
+        <v>12.408333333333333</v>
       </c>
       <c r="E42">
-        <v>290.25</v>
+        <v>251.47499999999999</v>
       </c>
       <c r="F42" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43">
-        <v>10000009</v>
+        <v>10000024</v>
       </c>
       <c r="B43" t="s">
-        <v>12</v>
+        <v>66</v>
       </c>
       <c r="C43" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="D43">
-        <v>14.708333333333334</v>
+        <v>12.125</v>
       </c>
       <c r="E43">
-        <v>300.75</v>
+        <v>249.25</v>
       </c>
       <c r="F43" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44">
-        <v>10000008</v>
+        <v>10000019</v>
       </c>
       <c r="B44" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="C44" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D44">
-        <v>15.833333333333334</v>
+        <v>12.458333333333334</v>
       </c>
       <c r="E44">
-        <v>320.25</v>
+        <v>242</v>
       </c>
       <c r="F44" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45">
-        <v>10000007</v>
+        <v>10000027</v>
       </c>
       <c r="B45" t="s">
-        <v>10</v>
+        <v>69</v>
       </c>
       <c r="C45" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="D45">
-        <v>13.733333333333334</v>
+        <v>12.033333333333333</v>
       </c>
       <c r="E45">
-        <v>273.57499999999999</v>
+        <v>238.5</v>
       </c>
       <c r="F45" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46">
-        <v>10000006</v>
+        <v>10000043</v>
       </c>
       <c r="B46" t="s">
-        <v>9</v>
+        <v>81</v>
       </c>
       <c r="C46" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="D46">
-        <v>14.878333333333332</v>
+        <v>11.958333333333334</v>
       </c>
       <c r="E46">
-        <v>294.81</v>
+        <v>237.875</v>
       </c>
       <c r="F46" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47">
-        <v>10000005</v>
+        <v>10000037</v>
       </c>
       <c r="B47" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
       <c r="C47" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D47">
-        <v>14.041666666666666</v>
+        <v>11.808333333333332</v>
       </c>
       <c r="E47">
-        <v>269.25</v>
+        <v>233.65</v>
       </c>
       <c r="F47" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48">
-        <v>10000004</v>
+        <v>10000042</v>
       </c>
       <c r="B48" t="s">
-        <v>7</v>
+        <v>80</v>
       </c>
       <c r="C48" t="s">
-        <v>26</v>
+        <v>59</v>
       </c>
       <c r="D48">
-        <v>12.366666666666667</v>
+        <v>12.049999999999999</v>
       </c>
       <c r="E48">
-        <v>267.39999999999998</v>
+        <v>231.4</v>
       </c>
       <c r="F48" t="s">
         <v>190</v>
@@ -9152,59 +9404,59 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50">
-        <v>10000002</v>
+        <v>10000036</v>
       </c>
       <c r="B50" t="s">
-        <v>5</v>
+        <v>75</v>
       </c>
       <c r="C50" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="D50">
-        <v>12.875</v>
+        <v>11.458333333333334</v>
       </c>
       <c r="E50">
-        <v>260.625</v>
+        <v>229.875</v>
       </c>
       <c r="F50" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51">
-        <v>10000001</v>
+        <v>10000000</v>
       </c>
       <c r="B51" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C51" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D51">
-        <v>14.208333333333334</v>
+        <v>11.166666666666666</v>
       </c>
       <c r="E51">
-        <v>288.125</v>
+        <v>217</v>
       </c>
       <c r="F51" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52">
-        <v>10000000</v>
+        <v>10000041</v>
       </c>
       <c r="B52" t="s">
-        <v>3</v>
+        <v>79</v>
       </c>
       <c r="C52" t="s">
-        <v>22</v>
+        <v>58</v>
       </c>
       <c r="D52">
-        <v>11.166666666666666</v>
+        <v>11.125</v>
       </c>
       <c r="E52">
-        <v>217</v>
+        <v>214.875</v>
       </c>
       <c r="F52" t="s">
         <v>190</v>
@@ -9212,19 +9464,19 @@
     </row>
   </sheetData>
   <sortState ref="A2:F52">
-    <sortCondition descending="1" ref="A1"/>
+    <sortCondition descending="1" ref="E1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0275A58-7EE0-4335-B98B-F043C997E23C}">
   <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9235,22 +9487,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="15" t="s">
         <v>173</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="15" t="s">
         <v>181</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="15" t="s">
         <v>184</v>
       </c>
     </row>
@@ -10255,6 +10507,1064 @@
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84BFE06F-D536-4F95-B89C-74C017646575}">
+  <dimension ref="A1:F52"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>173</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>183</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>10000252</v>
+      </c>
+      <c r="B2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>16.928571428571427</v>
+      </c>
+      <c r="E2">
+        <v>342.5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>10000257</v>
+      </c>
+      <c r="B3" t="s">
+        <v>202</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3">
+        <v>16.928571428571427</v>
+      </c>
+      <c r="E3">
+        <v>341.5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>10000285</v>
+      </c>
+      <c r="B4" t="s">
+        <v>203</v>
+      </c>
+      <c r="C4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4">
+        <v>15.964285714285714</v>
+      </c>
+      <c r="E4">
+        <v>319.125</v>
+      </c>
+      <c r="F4" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>10000286</v>
+      </c>
+      <c r="B5" t="s">
+        <v>204</v>
+      </c>
+      <c r="C5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D5">
+        <v>14.857142857142858</v>
+      </c>
+      <c r="E5">
+        <v>309</v>
+      </c>
+      <c r="F5" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>10000251</v>
+      </c>
+      <c r="B6" t="s">
+        <v>205</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>15.25</v>
+      </c>
+      <c r="E6">
+        <v>307.25</v>
+      </c>
+      <c r="F6" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>10000260</v>
+      </c>
+      <c r="B7" t="s">
+        <v>206</v>
+      </c>
+      <c r="C7" t="s">
+        <v>207</v>
+      </c>
+      <c r="D7">
+        <v>15.285714285714286</v>
+      </c>
+      <c r="E7">
+        <v>305</v>
+      </c>
+      <c r="F7" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>10000264</v>
+      </c>
+      <c r="B8" t="s">
+        <v>208</v>
+      </c>
+      <c r="C8" t="s">
+        <v>209</v>
+      </c>
+      <c r="D8">
+        <v>14.714285714285714</v>
+      </c>
+      <c r="E8">
+        <v>298.5</v>
+      </c>
+      <c r="F8" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>10000300</v>
+      </c>
+      <c r="B9" t="s">
+        <v>210</v>
+      </c>
+      <c r="C9" t="s">
+        <v>211</v>
+      </c>
+      <c r="D9">
+        <v>14.857142857142858</v>
+      </c>
+      <c r="E9">
+        <v>298</v>
+      </c>
+      <c r="F9" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>10000270</v>
+      </c>
+      <c r="B10" t="s">
+        <v>212</v>
+      </c>
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10">
+        <v>14.642857142857142</v>
+      </c>
+      <c r="E10">
+        <v>291.5</v>
+      </c>
+      <c r="F10" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10000288</v>
+      </c>
+      <c r="B11" t="s">
+        <v>213</v>
+      </c>
+      <c r="C11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D11">
+        <v>14.142857142857142</v>
+      </c>
+      <c r="E11">
+        <v>291.5</v>
+      </c>
+      <c r="F11" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>10000274</v>
+      </c>
+      <c r="B12" t="s">
+        <v>214</v>
+      </c>
+      <c r="C12" t="s">
+        <v>215</v>
+      </c>
+      <c r="D12">
+        <v>14.278571428571428</v>
+      </c>
+      <c r="E12">
+        <v>284.17500000000001</v>
+      </c>
+      <c r="F12" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>10000262</v>
+      </c>
+      <c r="B13" t="s">
+        <v>216</v>
+      </c>
+      <c r="C13" t="s">
+        <v>67</v>
+      </c>
+      <c r="D13">
+        <v>13.957142857142857</v>
+      </c>
+      <c r="E13">
+        <v>280.67500000000001</v>
+      </c>
+      <c r="F13" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>10000265</v>
+      </c>
+      <c r="B14" t="s">
+        <v>217</v>
+      </c>
+      <c r="C14" t="s">
+        <v>218</v>
+      </c>
+      <c r="D14">
+        <v>13.428571428571429</v>
+      </c>
+      <c r="E14">
+        <v>279</v>
+      </c>
+      <c r="F14" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>10000250</v>
+      </c>
+      <c r="B15" t="s">
+        <v>219</v>
+      </c>
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15">
+        <v>13.392857142857142</v>
+      </c>
+      <c r="E15">
+        <v>274.375</v>
+      </c>
+      <c r="F15" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>10000281</v>
+      </c>
+      <c r="B16" t="s">
+        <v>220</v>
+      </c>
+      <c r="C16" t="s">
+        <v>221</v>
+      </c>
+      <c r="D16">
+        <v>13.178571428571429</v>
+      </c>
+      <c r="E16">
+        <v>274.125</v>
+      </c>
+      <c r="F16" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>10000277</v>
+      </c>
+      <c r="B17" t="s">
+        <v>222</v>
+      </c>
+      <c r="C17" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17">
+        <v>13.678571428571429</v>
+      </c>
+      <c r="E17">
+        <v>273.125</v>
+      </c>
+      <c r="F17" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>10000289</v>
+      </c>
+      <c r="B18" t="s">
+        <v>223</v>
+      </c>
+      <c r="C18" t="s">
+        <v>224</v>
+      </c>
+      <c r="D18">
+        <v>13.142857142857142</v>
+      </c>
+      <c r="E18">
+        <v>271.75</v>
+      </c>
+      <c r="F18" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>10000283</v>
+      </c>
+      <c r="B19" t="s">
+        <v>225</v>
+      </c>
+      <c r="C19" t="s">
+        <v>226</v>
+      </c>
+      <c r="D19">
+        <v>13.392857142857142</v>
+      </c>
+      <c r="E19">
+        <v>271.125</v>
+      </c>
+      <c r="F19" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>10000268</v>
+      </c>
+      <c r="B20" t="s">
+        <v>227</v>
+      </c>
+      <c r="C20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20">
+        <v>13.071428571428571</v>
+      </c>
+      <c r="E20">
+        <v>267.125</v>
+      </c>
+      <c r="F20" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>10000276</v>
+      </c>
+      <c r="B21" t="s">
+        <v>229</v>
+      </c>
+      <c r="C21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21">
+        <v>13.357142857142858</v>
+      </c>
+      <c r="E21">
+        <v>266</v>
+      </c>
+      <c r="F21" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>10000259</v>
+      </c>
+      <c r="B22" t="s">
+        <v>230</v>
+      </c>
+      <c r="C22" t="s">
+        <v>231</v>
+      </c>
+      <c r="D22">
+        <v>13.321428571428571</v>
+      </c>
+      <c r="E22">
+        <v>263</v>
+      </c>
+      <c r="F22" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>10000263</v>
+      </c>
+      <c r="B23" t="s">
+        <v>232</v>
+      </c>
+      <c r="C23" t="s">
+        <v>233</v>
+      </c>
+      <c r="D23">
+        <v>13.207142857142857</v>
+      </c>
+      <c r="E23">
+        <v>262.77499999999998</v>
+      </c>
+      <c r="F23" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>10000253</v>
+      </c>
+      <c r="B24" t="s">
+        <v>234</v>
+      </c>
+      <c r="C24" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24">
+        <v>13.107142857142858</v>
+      </c>
+      <c r="E24">
+        <v>261.75</v>
+      </c>
+      <c r="F24" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>10000272</v>
+      </c>
+      <c r="B25" t="s">
+        <v>235</v>
+      </c>
+      <c r="C25" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25">
+        <v>12.785714285714286</v>
+      </c>
+      <c r="E25">
+        <v>260.75</v>
+      </c>
+      <c r="F25" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>10000256</v>
+      </c>
+      <c r="B26" t="s">
+        <v>236</v>
+      </c>
+      <c r="C26" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26">
+        <v>12.564285714285715</v>
+      </c>
+      <c r="E26">
+        <v>259.47500000000002</v>
+      </c>
+      <c r="F26" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>10000261</v>
+      </c>
+      <c r="B27" t="s">
+        <v>237</v>
+      </c>
+      <c r="C27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27">
+        <v>12.821428571428571</v>
+      </c>
+      <c r="E27">
+        <v>259.375</v>
+      </c>
+      <c r="F27" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>10000258</v>
+      </c>
+      <c r="B28" t="s">
+        <v>238</v>
+      </c>
+      <c r="C28" t="s">
+        <v>9</v>
+      </c>
+      <c r="D28">
+        <v>12.571428571428571</v>
+      </c>
+      <c r="E28">
+        <v>258.375</v>
+      </c>
+      <c r="F28" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>10000255</v>
+      </c>
+      <c r="B29" t="s">
+        <v>239</v>
+      </c>
+      <c r="C29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29">
+        <v>12.964285714285714</v>
+      </c>
+      <c r="E29">
+        <v>256.75</v>
+      </c>
+      <c r="F29" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>10000297</v>
+      </c>
+      <c r="B30" t="s">
+        <v>240</v>
+      </c>
+      <c r="C30" t="s">
+        <v>241</v>
+      </c>
+      <c r="D30">
+        <v>12.714285714285714</v>
+      </c>
+      <c r="E30">
+        <v>254.75</v>
+      </c>
+      <c r="F30" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>10000298</v>
+      </c>
+      <c r="B31" t="s">
+        <v>242</v>
+      </c>
+      <c r="C31" t="s">
+        <v>243</v>
+      </c>
+      <c r="D31">
+        <v>12.964285714285714</v>
+      </c>
+      <c r="E31">
+        <v>252.375</v>
+      </c>
+      <c r="F31" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>10000284</v>
+      </c>
+      <c r="B32" t="s">
+        <v>244</v>
+      </c>
+      <c r="C32" t="s">
+        <v>245</v>
+      </c>
+      <c r="D32">
+        <v>12.642857142857142</v>
+      </c>
+      <c r="E32">
+        <v>251.875</v>
+      </c>
+      <c r="F32" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>10000296</v>
+      </c>
+      <c r="B33" t="s">
+        <v>246</v>
+      </c>
+      <c r="C33" t="s">
+        <v>247</v>
+      </c>
+      <c r="D33">
+        <v>12.714285714285714</v>
+      </c>
+      <c r="E33">
+        <v>250.75</v>
+      </c>
+      <c r="F33" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>10000267</v>
+      </c>
+      <c r="B34" t="s">
+        <v>248</v>
+      </c>
+      <c r="C34" t="s">
+        <v>249</v>
+      </c>
+      <c r="D34">
+        <v>12.535714285714286</v>
+      </c>
+      <c r="E34">
+        <v>249.625</v>
+      </c>
+      <c r="F34" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>10000287</v>
+      </c>
+      <c r="B35" t="s">
+        <v>250</v>
+      </c>
+      <c r="C35" t="s">
+        <v>251</v>
+      </c>
+      <c r="D35">
+        <v>11.821428571428571</v>
+      </c>
+      <c r="E35">
+        <v>247</v>
+      </c>
+      <c r="F35" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>10000271</v>
+      </c>
+      <c r="B36" t="s">
+        <v>252</v>
+      </c>
+      <c r="C36" t="s">
+        <v>14</v>
+      </c>
+      <c r="D36">
+        <v>12.25</v>
+      </c>
+      <c r="E36">
+        <v>244.125</v>
+      </c>
+      <c r="F36" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>10000275</v>
+      </c>
+      <c r="B37" t="s">
+        <v>253</v>
+      </c>
+      <c r="C37" t="s">
+        <v>64</v>
+      </c>
+      <c r="D37">
+        <v>11.928571428571429</v>
+      </c>
+      <c r="E37">
+        <v>243.75</v>
+      </c>
+      <c r="F37" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>10000295</v>
+      </c>
+      <c r="B38" t="s">
+        <v>254</v>
+      </c>
+      <c r="C38" t="s">
+        <v>255</v>
+      </c>
+      <c r="D38">
+        <v>12.071428571428571</v>
+      </c>
+      <c r="E38">
+        <v>243.75</v>
+      </c>
+      <c r="F38" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>10000269</v>
+      </c>
+      <c r="B39" t="s">
+        <v>256</v>
+      </c>
+      <c r="C39" t="s">
+        <v>70</v>
+      </c>
+      <c r="D39">
+        <v>12.1</v>
+      </c>
+      <c r="E39">
+        <v>242.1</v>
+      </c>
+      <c r="F39" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>10000266</v>
+      </c>
+      <c r="B40" t="s">
+        <v>257</v>
+      </c>
+      <c r="C40" t="s">
+        <v>258</v>
+      </c>
+      <c r="D40">
+        <v>12</v>
+      </c>
+      <c r="E40">
+        <v>241</v>
+      </c>
+      <c r="F40" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>10000294</v>
+      </c>
+      <c r="B41" t="s">
+        <v>259</v>
+      </c>
+      <c r="C41" t="s">
+        <v>260</v>
+      </c>
+      <c r="D41">
+        <v>11.607142857142858</v>
+      </c>
+      <c r="E41">
+        <v>236.625</v>
+      </c>
+      <c r="F41" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>10000282</v>
+      </c>
+      <c r="B42" t="s">
+        <v>261</v>
+      </c>
+      <c r="C42" t="s">
+        <v>262</v>
+      </c>
+      <c r="D42">
+        <v>11.642857142857142</v>
+      </c>
+      <c r="E42">
+        <v>233.75</v>
+      </c>
+      <c r="F42" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>10000280</v>
+      </c>
+      <c r="B43" t="s">
+        <v>263</v>
+      </c>
+      <c r="C43" t="s">
+        <v>264</v>
+      </c>
+      <c r="D43">
+        <v>11.642857142857142</v>
+      </c>
+      <c r="E43">
+        <v>233</v>
+      </c>
+      <c r="F43" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>10000254</v>
+      </c>
+      <c r="B44" t="s">
+        <v>266</v>
+      </c>
+      <c r="C44" t="s">
+        <v>7</v>
+      </c>
+      <c r="D44">
+        <v>11.778571428571428</v>
+      </c>
+      <c r="E44">
+        <v>231.15</v>
+      </c>
+      <c r="F44" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>10000279</v>
+      </c>
+      <c r="B45" t="s">
+        <v>267</v>
+      </c>
+      <c r="C45" t="s">
+        <v>21</v>
+      </c>
+      <c r="D45">
+        <v>11.5</v>
+      </c>
+      <c r="E45">
+        <v>230.25</v>
+      </c>
+      <c r="F45" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>10000290</v>
+      </c>
+      <c r="B46" t="s">
+        <v>268</v>
+      </c>
+      <c r="C46" t="s">
+        <v>235</v>
+      </c>
+      <c r="D46">
+        <v>11.285714285714286</v>
+      </c>
+      <c r="E46">
+        <v>224</v>
+      </c>
+      <c r="F46" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>10000299</v>
+      </c>
+      <c r="B47" t="s">
+        <v>269</v>
+      </c>
+      <c r="C47" t="s">
+        <v>270</v>
+      </c>
+      <c r="D47">
+        <v>11.492857142857144</v>
+      </c>
+      <c r="E47">
+        <v>222.77500000000001</v>
+      </c>
+      <c r="F47" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>10000278</v>
+      </c>
+      <c r="B48" t="s">
+        <v>271</v>
+      </c>
+      <c r="C48" t="s">
+        <v>20</v>
+      </c>
+      <c r="D48">
+        <v>11.25</v>
+      </c>
+      <c r="E48">
+        <v>222</v>
+      </c>
+      <c r="F48" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>10000293</v>
+      </c>
+      <c r="B49" t="s">
+        <v>272</v>
+      </c>
+      <c r="C49" t="s">
+        <v>273</v>
+      </c>
+      <c r="D49">
+        <v>10.892857142857142</v>
+      </c>
+      <c r="E49">
+        <v>217.125</v>
+      </c>
+      <c r="F49" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>10000273</v>
+      </c>
+      <c r="B50" t="s">
+        <v>107</v>
+      </c>
+      <c r="C50" t="s">
+        <v>17</v>
+      </c>
+      <c r="D50">
+        <v>10.857142857142858</v>
+      </c>
+      <c r="E50">
+        <v>217</v>
+      </c>
+      <c r="F50" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>10000291</v>
+      </c>
+      <c r="B51" t="s">
+        <v>274</v>
+      </c>
+      <c r="C51" t="s">
+        <v>96</v>
+      </c>
+      <c r="D51">
+        <v>11</v>
+      </c>
+      <c r="E51">
+        <v>216.375</v>
+      </c>
+      <c r="F51" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>10000292</v>
+      </c>
+      <c r="B52" t="s">
+        <v>96</v>
+      </c>
+      <c r="C52" t="s">
+        <v>275</v>
+      </c>
+      <c r="D52">
+        <v>10.785714285714286</v>
+      </c>
+      <c r="E52">
+        <v>214.375</v>
+      </c>
+      <c r="F52" t="s">
+        <v>265</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A2:F52">
+    <sortCondition descending="1" ref="E1"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>